<commit_message>
fix retrofit and random tornado with excel
</commit_message>
<xml_diff>
--- a/Table3-fixRetrofitted.xlsx
+++ b/Table3-fixRetrofitted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F4E66-EDF4-44DA-A54C-7D240D659C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA9D205-247F-45C3-A5F5-26AD8DF65327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>Base Case</t>
+    <t>Base Case (Original Formulation)</t>
   </si>
 </sst>
 </file>
@@ -387,15 +387,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -411,9 +402,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,14 +411,26 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1205,7 +1205,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1277,45 +1277,45 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>16313</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>16318</v>
       </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
         <v>199.97</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <v>2</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>199.74</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>36</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <v>7.13</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="9">
         <v>14</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="10">
         <v>2.54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="18" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="6">
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -1389,7 +1389,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2">
         <v>3</v>
       </c>
@@ -1425,53 +1425,53 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <f>AVERAGE(C6:C8)</f>
         <v>16114.666666666666</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <f t="shared" ref="D9:L9" si="0">AVERAGE(D6:D8)</f>
         <v>16174.333333333334</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>150.08333333333334</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <f t="shared" si="0"/>
         <v>149.83333333333334</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <f t="shared" si="0"/>
         <v>39.666666666666664</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="9">
         <f t="shared" si="0"/>
         <v>9.0299999999999994</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="9">
         <f t="shared" si="0"/>
         <v>15.666666666666666</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="10">
         <f t="shared" si="0"/>
         <v>4.3133333333333335</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="6">
@@ -1509,7 +1509,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="8"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="2">
         <v>2</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="8"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="2">
         <v>3</v>
       </c>
@@ -1581,53 +1581,53 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="9"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <f>AVERAGE(C10:C12)</f>
         <v>15688</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <f t="shared" ref="D13:L13" si="1">AVERAGE(D10:D12)</f>
         <v>15694</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <f t="shared" si="1"/>
         <v>125.74333333333334</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="9">
         <f t="shared" si="1"/>
         <v>125.58999999999999</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="9">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="9">
         <f t="shared" si="1"/>
         <v>5.0200000000000005</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="9">
         <f t="shared" si="1"/>
         <v>12.666666666666666</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="10">
         <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="6">
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="2">
         <v>2</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="8"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="2">
         <v>3</v>
       </c>
@@ -1737,15 +1737,15 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="8"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <f>AVERAGE(C14:C16)</f>
         <v>15167</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="15">
         <f t="shared" ref="D17:L17" si="2">AVERAGE(D14:D16)</f>
         <v>15167</v>
       </c>
@@ -1777,44 +1777,44 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="15">
         <f t="shared" si="2"/>
         <v>1.2466666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21">
+      <c r="B18" s="22"/>
+      <c r="C18" s="16">
         <v>13312</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="17">
         <v>13408</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>0.01</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="9">
         <v>306.77</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="9">
         <v>3</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="9">
         <v>306.41000000000003</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>69</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="9">
         <v>11.23</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="9">
         <v>29</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="10">
         <v>5.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new results for fixed tornado
</commit_message>
<xml_diff>
--- a/Table3-fixRetrofitted.xlsx
+++ b/Table3-fixRetrofitted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2100409F-ECA8-43A3-AA53-D48B88D0455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D254DA-0ACF-442D-896D-8B4371DDEF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,18 +26,26 @@
     <sheet name="15M-3" sheetId="7" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Summary!$P$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Summary!$A$20</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Summary!$D$6:$D$15</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Summary!$P$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Summary!$A$34</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Summary!$A$48</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Summary!$A$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Summary!$A$6</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Summary!$D$20:$D$29</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Summary!$D$34:$D$43</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Summary!$D$48</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Summary!$D$5</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Summary!$A$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Summary!$A$34</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Summary!$A$20</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Summary!$A$34</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Summary!$A$48</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Summary!$A$5</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Summary!$A$6</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Summary!$D$20:$D$29</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Summary!$D$34:$D$43</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Summary!$D$48</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Summary!$D$5</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Summary!$D$6:$D$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Summary!$A$48</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Summary!$A$5</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Summary!$A$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Summary!$D$20:$D$29</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Summary!$D$34:$D$43</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Summary!$D$48</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Summary!$D$5</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Summary!$D$6:$D$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -456,21 +464,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -487,6 +480,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,38 +519,37 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{993409C8-CCFD-48ED-B569-B58CD4DD4EBA}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.3</cx:f>
               <cx:v>0%/0M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -555,7 +562,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-5730-48CF-9A03-1F61E469D48A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.5</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>20%/3M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -567,7 +574,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000002-5730-48CF-9A03-1F61E469D48A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>60%/9M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -579,7 +586,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000003-5730-48CF-9A03-1F61E469D48A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>100%/15M</cx:v>
             </cx:txData>
           </cx:tx>
@@ -591,7 +598,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{00000004-5730-48CF-9A03-1F61E469D48A}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.3</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>Base Case (Original Formulation)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -603,10 +610,66 @@
       </cx:plotAreaRegion>
       <cx:axis id="0">
         <cx:catScaling gapWidth="1"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Budget to Retrofit</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Budget to Retrofit</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:tickLabels/>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling max="16500" min="13000"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Population Dislocation</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Population Dislocation</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
         <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
@@ -1219,8 +1282,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11093824" y="2408517"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="11087100" y="2373779"/>
+              <a:ext cx="4551083" cy="2700617"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2009,7 +2072,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2119,7 +2182,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="34" t="s">
         <v>41</v>
       </c>
       <c r="B6" s="14">
@@ -2157,7 +2220,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="15">
         <v>2</v>
       </c>
@@ -2193,7 +2256,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="15">
         <v>3</v>
       </c>
@@ -2229,259 +2292,259 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="15">
         <v>4</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="28">
         <v>16080</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="29">
         <v>16097</v>
       </c>
-      <c r="E9" s="33">
-        <v>0</v>
-      </c>
-      <c r="F9" s="37">
+      <c r="E9" s="28">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
         <v>129.15</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="32">
         <v>2</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="32">
         <v>128.99</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="32">
         <v>40</v>
       </c>
-      <c r="J9" s="37">
+      <c r="J9" s="32">
         <v>8.73</v>
       </c>
-      <c r="K9" s="37">
+      <c r="K9" s="32">
         <v>19</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="29">
         <v>5.0199999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="15">
         <v>5</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="28">
         <v>15845</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="29">
         <v>15904</v>
       </c>
-      <c r="E10" s="33">
-        <v>0</v>
-      </c>
-      <c r="F10" s="37">
+      <c r="E10" s="28">
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
         <v>165.9</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="32">
         <v>2</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="32">
         <v>165.68</v>
       </c>
-      <c r="I10" s="37">
+      <c r="I10" s="32">
         <v>39</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="32">
         <v>7.53</v>
       </c>
-      <c r="K10" s="37">
+      <c r="K10" s="32">
         <v>15</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="29">
         <v>2.15</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="15">
         <v>6</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="28">
         <v>16037</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="29">
         <v>16120</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="28">
         <v>0.01</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="32">
         <v>183.32</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="32">
         <v>2</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="32">
         <v>183.11</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="32">
         <v>44</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="32">
         <v>9.11</v>
       </c>
-      <c r="K11" s="37">
+      <c r="K11" s="32">
         <v>16</v>
       </c>
-      <c r="L11" s="34">
+      <c r="L11" s="29">
         <v>3.74</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="15">
         <v>7</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="28">
         <v>16215</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="29">
         <v>16218</v>
       </c>
-      <c r="E12" s="33">
-        <v>0</v>
-      </c>
-      <c r="F12" s="37">
+      <c r="E12" s="28">
+        <v>0</v>
+      </c>
+      <c r="F12" s="32">
         <v>153.03</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="32">
         <v>2</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="32">
         <v>152.85</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="32">
         <v>26</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="32">
         <v>3.83</v>
       </c>
-      <c r="K12" s="37">
+      <c r="K12" s="32">
         <v>8</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="29">
         <v>1.31</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="15">
         <v>8</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="28">
         <v>15717</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="29">
         <v>15717</v>
       </c>
-      <c r="E13" s="33">
-        <v>0</v>
-      </c>
-      <c r="F13" s="37">
+      <c r="E13" s="28">
+        <v>0</v>
+      </c>
+      <c r="F13" s="32">
         <v>151.63999999999999</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="32">
         <v>2</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="32">
         <v>151.44999999999999</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="32">
         <v>37</v>
       </c>
-      <c r="J13" s="37">
+      <c r="J13" s="32">
         <v>6.27</v>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="32">
         <v>19</v>
       </c>
-      <c r="L13" s="34">
+      <c r="L13" s="29">
         <v>2.09</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="15">
         <v>9</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="28">
         <v>16005</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="29">
         <v>16005</v>
       </c>
-      <c r="E14" s="33">
-        <v>0</v>
-      </c>
-      <c r="F14" s="37">
+      <c r="E14" s="28">
+        <v>0</v>
+      </c>
+      <c r="F14" s="32">
         <v>154.97</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="32">
         <v>2</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="32">
         <v>154.78</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="32">
         <v>26</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="32">
         <v>4.1900000000000004</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="32">
         <v>5</v>
       </c>
-      <c r="L14" s="34">
+      <c r="L14" s="29">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="29"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="16">
         <v>10</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="30">
         <v>15990</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="31">
         <v>15990</v>
       </c>
-      <c r="E15" s="35">
-        <v>0</v>
-      </c>
-      <c r="F15" s="38">
+      <c r="E15" s="30">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33">
         <v>171.58</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="33">
         <v>2</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="33">
         <v>171.37</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="33">
         <v>40</v>
       </c>
-      <c r="J15" s="38">
+      <c r="J15" s="33">
         <v>6.61</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="33">
         <v>16</v>
       </c>
-      <c r="L15" s="36">
+      <c r="L15" s="31">
         <v>2.73</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -2519,7 +2582,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="29"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="20" t="s">
         <v>49</v>
       </c>
@@ -2557,7 +2620,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="21" t="s">
         <v>45</v>
       </c>
@@ -2603,7 +2666,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="30"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="20" t="s">
         <v>50</v>
       </c>
@@ -2649,7 +2712,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="34" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="14">
@@ -2687,7 +2750,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21" s="29"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="15">
         <v>2</v>
       </c>
@@ -2723,7 +2786,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" s="29"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="15">
         <v>3</v>
       </c>
@@ -2759,259 +2822,259 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="15">
         <v>4</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="28">
         <v>15722</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="29">
         <v>15723</v>
       </c>
-      <c r="E23" s="33">
-        <v>0</v>
-      </c>
-      <c r="F23" s="37">
+      <c r="E23" s="28">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
         <v>154.18</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="32">
         <v>2</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="32">
         <v>153.97</v>
       </c>
-      <c r="I23" s="37">
+      <c r="I23" s="32">
         <v>35</v>
       </c>
-      <c r="J23" s="37">
+      <c r="J23" s="32">
         <v>5.4</v>
       </c>
-      <c r="K23" s="37">
+      <c r="K23" s="32">
         <v>12</v>
       </c>
-      <c r="L23" s="34">
+      <c r="L23" s="29">
         <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24" s="29"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="15">
         <v>5</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="28">
         <v>15305</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="29">
         <v>15306</v>
       </c>
-      <c r="E24" s="33">
-        <v>0</v>
-      </c>
-      <c r="F24" s="37">
+      <c r="E24" s="28">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
         <v>149.04</v>
       </c>
-      <c r="G24" s="37">
+      <c r="G24" s="32">
         <v>2</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="32">
         <v>148.75</v>
       </c>
-      <c r="I24" s="37">
+      <c r="I24" s="32">
         <v>39</v>
       </c>
-      <c r="J24" s="37">
+      <c r="J24" s="32">
         <v>6.19</v>
       </c>
-      <c r="K24" s="37">
+      <c r="K24" s="32">
         <v>12</v>
       </c>
-      <c r="L24" s="34">
+      <c r="L24" s="29">
         <v>2.2799999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="15">
         <v>6</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="28">
         <v>15615</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="29">
         <v>15645</v>
       </c>
-      <c r="E25" s="33">
-        <v>0</v>
-      </c>
-      <c r="F25" s="37">
+      <c r="E25" s="28">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
         <v>155.28</v>
       </c>
-      <c r="G25" s="37">
+      <c r="G25" s="32">
         <v>2</v>
       </c>
-      <c r="H25" s="37">
+      <c r="H25" s="32">
         <v>154.99</v>
       </c>
-      <c r="I25" s="37">
+      <c r="I25" s="32">
         <v>48</v>
       </c>
-      <c r="J25" s="37">
+      <c r="J25" s="32">
         <v>8.5500000000000007</v>
       </c>
-      <c r="K25" s="37">
+      <c r="K25" s="32">
         <v>16</v>
       </c>
-      <c r="L25" s="34">
+      <c r="L25" s="29">
         <v>2.92</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="15">
         <v>7</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="28">
         <v>15634</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="29">
         <v>15635</v>
       </c>
-      <c r="E26" s="33">
-        <v>0</v>
-      </c>
-      <c r="F26" s="37">
+      <c r="E26" s="28">
+        <v>0</v>
+      </c>
+      <c r="F26" s="32">
         <v>136.66999999999999</v>
       </c>
-      <c r="G26" s="37">
+      <c r="G26" s="32">
         <v>2</v>
       </c>
-      <c r="H26" s="37">
+      <c r="H26" s="32">
         <v>136.37</v>
       </c>
-      <c r="I26" s="37">
+      <c r="I26" s="32">
         <v>40</v>
       </c>
-      <c r="J26" s="37">
+      <c r="J26" s="32">
         <v>6.5</v>
       </c>
-      <c r="K26" s="37">
+      <c r="K26" s="32">
         <v>12</v>
       </c>
-      <c r="L26" s="34">
+      <c r="L26" s="29">
         <v>1.84</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="15">
         <v>8</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="28">
         <v>15444</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="29">
         <v>15474</v>
       </c>
-      <c r="E27" s="33">
-        <v>0</v>
-      </c>
-      <c r="F27" s="37">
+      <c r="E27" s="28">
+        <v>0</v>
+      </c>
+      <c r="F27" s="32">
         <v>150.79</v>
       </c>
-      <c r="G27" s="37">
+      <c r="G27" s="32">
         <v>2</v>
       </c>
-      <c r="H27" s="37">
+      <c r="H27" s="32">
         <v>150.57</v>
       </c>
-      <c r="I27" s="37">
+      <c r="I27" s="32">
         <v>42</v>
       </c>
-      <c r="J27" s="37">
+      <c r="J27" s="32">
         <v>6.59</v>
       </c>
-      <c r="K27" s="37">
+      <c r="K27" s="32">
         <v>11</v>
       </c>
-      <c r="L27" s="34">
+      <c r="L27" s="29">
         <v>2.06</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="15">
         <v>9</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="28">
         <v>15703</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="29">
         <v>15704</v>
       </c>
-      <c r="E28" s="33">
-        <v>0</v>
-      </c>
-      <c r="F28" s="37">
+      <c r="E28" s="28">
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
         <v>211.05</v>
       </c>
-      <c r="G28" s="37">
+      <c r="G28" s="32">
         <v>2</v>
       </c>
-      <c r="H28" s="37">
+      <c r="H28" s="32">
         <v>210.73</v>
       </c>
-      <c r="I28" s="37">
+      <c r="I28" s="32">
         <v>40</v>
       </c>
-      <c r="J28" s="37">
+      <c r="J28" s="32">
         <v>7.53</v>
       </c>
-      <c r="K28" s="37">
+      <c r="K28" s="32">
         <v>9</v>
       </c>
-      <c r="L28" s="34">
+      <c r="L28" s="29">
         <v>2.42</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="29"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="16">
         <v>10</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="30">
         <v>15305</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="31">
         <v>15392</v>
       </c>
-      <c r="E29" s="35">
+      <c r="E29" s="30">
         <v>0.01</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="33">
         <v>214.42</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="33">
         <v>2</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="33">
         <v>214.17</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="33">
         <v>51</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J29" s="33">
         <v>12.68</v>
       </c>
-      <c r="K29" s="38">
+      <c r="K29" s="33">
         <v>13</v>
       </c>
-      <c r="L29" s="36">
+      <c r="L29" s="31">
         <v>5.41</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="17" t="s">
         <v>48</v>
       </c>
@@ -3049,7 +3112,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="29"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="20" t="s">
         <v>49</v>
       </c>
@@ -3087,7 +3150,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="21" t="s">
         <v>45</v>
       </c>
@@ -3133,7 +3196,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="30"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="20" t="s">
         <v>50</v>
       </c>
@@ -3179,7 +3242,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="14">
@@ -3217,7 +3280,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="29"/>
+      <c r="A35" s="35"/>
       <c r="B35" s="15">
         <v>2</v>
       </c>
@@ -3253,7 +3316,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A36" s="29"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="15">
         <v>3</v>
       </c>
@@ -3289,259 +3352,259 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A37" s="29"/>
+      <c r="A37" s="35"/>
       <c r="B37" s="15">
         <v>4</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C37" s="28">
         <v>14764</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="29">
         <v>14764</v>
       </c>
-      <c r="E37" s="33">
-        <v>0</v>
-      </c>
-      <c r="F37" s="37">
+      <c r="E37" s="28">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
         <v>235.78</v>
       </c>
-      <c r="G37" s="37">
+      <c r="G37" s="32">
         <v>2</v>
       </c>
-      <c r="H37" s="37">
+      <c r="H37" s="32">
         <v>235.36</v>
       </c>
-      <c r="I37" s="37">
+      <c r="I37" s="32">
         <v>42</v>
       </c>
-      <c r="J37" s="37">
+      <c r="J37" s="32">
         <v>8.25</v>
       </c>
-      <c r="K37" s="37">
+      <c r="K37" s="32">
         <v>15</v>
       </c>
-      <c r="L37" s="34">
+      <c r="L37" s="29">
         <v>2.4</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A38" s="29"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="15">
         <v>5</v>
       </c>
-      <c r="C38" s="33">
+      <c r="C38" s="28">
         <v>15069</v>
       </c>
-      <c r="D38" s="34">
+      <c r="D38" s="29">
         <v>15069</v>
       </c>
-      <c r="E38" s="33">
-        <v>0</v>
-      </c>
-      <c r="F38" s="37">
+      <c r="E38" s="28">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
         <v>165.88</v>
       </c>
-      <c r="G38" s="37">
+      <c r="G38" s="32">
         <v>2</v>
       </c>
-      <c r="H38" s="37">
+      <c r="H38" s="32">
         <v>165.65</v>
       </c>
-      <c r="I38" s="37">
+      <c r="I38" s="32">
         <v>38</v>
       </c>
-      <c r="J38" s="37">
+      <c r="J38" s="32">
         <v>6.93</v>
       </c>
-      <c r="K38" s="37">
+      <c r="K38" s="32">
         <v>6</v>
       </c>
-      <c r="L38" s="34">
+      <c r="L38" s="29">
         <v>2.2200000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A39" s="29"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="15">
         <v>6</v>
       </c>
-      <c r="C39" s="33">
+      <c r="C39" s="28">
         <v>15451</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="29">
         <v>15451</v>
       </c>
-      <c r="E39" s="33">
-        <v>0</v>
-      </c>
-      <c r="F39" s="37">
+      <c r="E39" s="28">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
         <v>158.88</v>
       </c>
-      <c r="G39" s="37">
+      <c r="G39" s="32">
         <v>2</v>
       </c>
-      <c r="H39" s="37">
+      <c r="H39" s="32">
         <v>158.65</v>
       </c>
-      <c r="I39" s="37">
+      <c r="I39" s="32">
         <v>30</v>
       </c>
-      <c r="J39" s="37">
+      <c r="J39" s="32">
         <v>5.17</v>
       </c>
-      <c r="K39" s="37">
+      <c r="K39" s="32">
         <v>6</v>
       </c>
-      <c r="L39" s="34">
+      <c r="L39" s="29">
         <v>1.52</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A40" s="29"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="15">
         <v>7</v>
       </c>
-      <c r="C40" s="33">
+      <c r="C40" s="28">
         <v>15378</v>
       </c>
-      <c r="D40" s="34">
+      <c r="D40" s="29">
         <v>15378</v>
       </c>
-      <c r="E40" s="33">
-        <v>0</v>
-      </c>
-      <c r="F40" s="37">
+      <c r="E40" s="28">
+        <v>0</v>
+      </c>
+      <c r="F40" s="32">
         <v>188.59</v>
       </c>
-      <c r="G40" s="37">
+      <c r="G40" s="32">
         <v>2</v>
       </c>
-      <c r="H40" s="37">
+      <c r="H40" s="32">
         <v>188.3</v>
       </c>
-      <c r="I40" s="37">
+      <c r="I40" s="32">
         <v>36</v>
       </c>
-      <c r="J40" s="37">
+      <c r="J40" s="32">
         <v>9.35</v>
       </c>
-      <c r="K40" s="37">
+      <c r="K40" s="32">
         <v>12</v>
       </c>
-      <c r="L40" s="34">
+      <c r="L40" s="29">
         <v>2.77</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A41" s="29"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="15">
         <v>8</v>
       </c>
-      <c r="C41" s="33">
+      <c r="C41" s="28">
         <v>15058</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="29">
         <v>15058</v>
       </c>
-      <c r="E41" s="33">
-        <v>0</v>
-      </c>
-      <c r="F41" s="37">
+      <c r="E41" s="28">
+        <v>0</v>
+      </c>
+      <c r="F41" s="32">
         <v>152.04</v>
       </c>
-      <c r="G41" s="37">
+      <c r="G41" s="32">
         <v>2</v>
       </c>
-      <c r="H41" s="37">
+      <c r="H41" s="32">
         <v>151.81</v>
       </c>
-      <c r="I41" s="37">
+      <c r="I41" s="32">
         <v>42</v>
       </c>
-      <c r="J41" s="37">
+      <c r="J41" s="32">
         <v>8.99</v>
       </c>
-      <c r="K41" s="37">
+      <c r="K41" s="32">
         <v>22</v>
       </c>
-      <c r="L41" s="34">
+      <c r="L41" s="29">
         <v>4.1100000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A42" s="29"/>
+      <c r="A42" s="35"/>
       <c r="B42" s="15">
         <v>9</v>
       </c>
-      <c r="C42" s="33">
+      <c r="C42" s="28">
         <v>15005</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="29">
         <v>15005</v>
       </c>
-      <c r="E42" s="33">
-        <v>0</v>
-      </c>
-      <c r="F42" s="37">
+      <c r="E42" s="28">
+        <v>0</v>
+      </c>
+      <c r="F42" s="32">
         <v>221.14</v>
       </c>
-      <c r="G42" s="37">
+      <c r="G42" s="32">
         <v>2</v>
       </c>
-      <c r="H42" s="37">
+      <c r="H42" s="32">
         <v>220.82</v>
       </c>
-      <c r="I42" s="37">
+      <c r="I42" s="32">
         <v>39</v>
       </c>
-      <c r="J42" s="37">
+      <c r="J42" s="32">
         <v>9.32</v>
       </c>
-      <c r="K42" s="37">
+      <c r="K42" s="32">
         <v>17</v>
       </c>
-      <c r="L42" s="34">
+      <c r="L42" s="29">
         <v>3.46</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="29"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="15">
         <v>10</v>
       </c>
-      <c r="C43" s="35">
+      <c r="C43" s="30">
         <v>15203</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="31">
         <v>15203</v>
       </c>
-      <c r="E43" s="35">
-        <v>0</v>
-      </c>
-      <c r="F43" s="38">
+      <c r="E43" s="30">
+        <v>0</v>
+      </c>
+      <c r="F43" s="33">
         <v>150.74</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="33">
         <v>2</v>
       </c>
-      <c r="H43" s="38">
+      <c r="H43" s="33">
         <v>150.38</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I43" s="33">
         <v>35</v>
       </c>
-      <c r="J43" s="38">
+      <c r="J43" s="33">
         <v>8.6999999999999993</v>
       </c>
-      <c r="K43" s="38">
+      <c r="K43" s="33">
         <v>15</v>
       </c>
-      <c r="L43" s="36">
+      <c r="L43" s="31">
         <v>3.36</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" s="29"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="17" t="s">
         <v>48</v>
       </c>
@@ -3579,7 +3642,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="29"/>
+      <c r="A45" s="35"/>
       <c r="B45" s="20" t="s">
         <v>49</v>
       </c>
@@ -3617,7 +3680,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A46" s="29"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="21" t="s">
         <v>45</v>
       </c>
@@ -3663,7 +3726,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="30"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="20" t="s">
         <v>50</v>
       </c>
@@ -3709,10 +3772,10 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="32"/>
+      <c r="B48" s="38"/>
       <c r="C48" s="25">
         <v>13312</v>
       </c>

</xml_diff>